<commit_message>
Refactor and enhance the unified scraper system. Updated README to reflect new features and installation instructions. Adjusted PDF export formatting and temporarily disabled PDF output due to issues. Improved job scraping logic for Y Combinator, focusing on internships and remote roles, and enhanced pay extraction methods. Updated state management to track known job listings more effectively.
</commit_message>
<xml_diff>
--- a/startup-intern-scraper/out/internships.xlsx
+++ b/startup-intern-scraper/out/internships.xlsx
@@ -493,7 +493,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>43437c1147e05629b0d7444a7a97c70fbcd465058df4f339deb4c6fd9b795075</t>
+          <t>8afdb4c548ccc924f17baf60ddeea7eb36d0fdeae2bf326e54da8d48dd931768</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -508,7 +508,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Principal Full-Stack Engineer (Django)</t>
+          <t>Senior Data Engineer</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -516,29 +516,33 @@
           <t>San Francisco - Remote / Remote (US)</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>AboutWhat Happens at YC?ApplyYC Interview GuideFAQPeopleYC BlogCompaniesStartup DirectoryFounder DirectoryLaunch YCStartup JobsAll Jobs◦ Engineering◦ Operations◦ Marketing◦ SalesInternshipsStartup Job GuideYC Startup Jobs BlogFind a Co-FounderLibrarySAFEResourcesStartup SchoolNewsletterRequests for StartupsFor InvestorsVerify FoundersHacker NewsBookfaceOpen main menuApply forW2026batch.ApplyVerge GenomicsWe use human data and AI to develop better drugs faster.Senior Data Engineer•San Francisco - Remote / Remote (US)Job typeFull-timeRoleEngineering, Full stackVisaUS citizen/visa onlyApply toVerge Genomicsand hundreds of other fast-growing YC startups with a single profile.Apply to role ›About the roleWho We AreTechnology has transformed every aspect of our lives. Yet, it still takes 12 years to develop a single drug because 90% of drugs fail in clinical trials, leaving hundreds of millions of patients without effective treatments. Accelerating the pace of bringing new, effective medicines to patients is one of the greatest opportunities for humanity.Our mission is to develop better drugs, faster using artificial intelligence (AI) and human data. We have created a proprietary, all-in-human AI drug discovery engine, CONVERGE, which houses one of the field's largest and most comprehensive databases of multi-modal patient data sourced directly from human tissue. We use machine learning to map the complex causes of disease, discover new targets with a greater probability of success, and de-risk drug development.We have delivered 2 new drugs from CONVERGE to clinical trials, discovered 282 new targets, and signed 2 commercial partnerships with Eli Lilly and AstraZeneca totaling $1.6B. We are a team of engineers, neuroscientists, and drug developers united around an audacious vision: to build the Genentech of the digital age.Your MissionReporting to the Head of Product &amp; Engineering, and working alongside Verge's platform and computational biology teams, the Senior Data Engineer will transform existing infrastructure into a highly scalable data platform that unlocks faster, easier access to data for both internal teams and external customers, while serving as a robust foundation for rapidly deploying new data products and SaaS capabilities.Your 12 Month OutcomesFully automated internal target discovery analysis tooling built and operational, serving the team providing target discovery services to external customers,Data pipeline and infrastructure launched to power self-serve MVP built on top of CONVERGE, allowing external customers to pay for and use Verge's bespoke dataset and tools to unlock transformative insights.You WillDesign and build scalable data infrastructure to support a multi-tenanted Biotech data and analysis platform,Architect data pipelines that handle diverse scientific data sources and formats,Develop APIs and integration points for data ingestion and export,Implement robust data processing workflows using modern frameworks (Apache Spark, Kafka, Airflow, etc.),Lead technical migration from single-tenant internal tool to multi-tenant SaaS platform,Create self-service capabilities including user dashboards, data exploration tools, and automated reporting,Set up cloud infrastructure (AWS/GCP/Azure) with focus on scalability and cost optimization,Implement CI/CD pipelines for data platform deployments,Build customer-facing data tools and visualization capabilities,Create data quality monitoring and validation systems.RequirementsCandidatesmust have:4+ years of experience in data engineering with hands-on pipeline development,Strong proficiency in Python and SQL,Experience with cloud platforms (AWS, GCP, or Azure) and infrastructure-as-code tools,Proven experience with distributed data processing frameworks (Spark, Kafka, Flink),Solid understanding of database technologies (PostgreSQL, MongoDB, Redis, data warehouses, graph databases),Experience with containerization (Docker, Kubernetes) and orchestration tools,Previous experience building and scaling SaaS applications,Understanding of multi-tenant architecture patterns and data isolation strategies,Experience with API design and development for external customers,Strong background in performance optimization and troubleshooting,Experience with automated testing frameworks for data pipelines.Exceptional candidateswill also have:Previous experience as a founding or early-stage engineer at a data/analytics company,Background in machine learning/statistical modelling,Knowledge of data visualization tools and customer-facing analytics,Experience building full-stack web applications in Django, and opinions on how to build intuitive front-ends,Academic or professional experience in biology, genomics, or a related field.Finally, we seek candidates who embrace our values and way of working:Ability to thrive in uncertainty with frequently changing prioritiesDeep alignment withour valuesA passion for making an impact on patientsAboutVerge GenomicsTechnology has transformed every aspect of our lives. Yet, it still takes 12 years to develop a single drug because 90% of drugs fail in clinical trials, leaving hundreds of millions of patients without effective treatments. Accelerating the pace of bringing new, effective medicines to patients is one of the greatest opportunities for humanity.Our mission is to develop better drugs, faster using artificial intelligence (AI) and human data. We have created a proprietary, all-in-human AI drug discovery engine, CONVERGE, which houses one of the field's largest and most comprehensive databases of multi-modal patient data sourced directly from human tissue. We use machine learning to map the complex causes of disease, discover new targets with a greater probability of success, and de-risk drug development.We have delivered 2 new drugs from CONVERGE to clinical trials, discovered 282 new targets, and signed 2 commercial partnerships with Eli Lilly and AstraZeneca totaling $1.6B. We are a team of engineers, neuroscientists, and drug developers united around an audacious vision: to build the Genentech of the digital age.Verge GenomicsFounded:2015Batch:S15Team Size:50Status:ActiveFoundersAlice ZhangCEOAlice ZhangCEOSimilar JobsEkhoFull-stack EngineerGatherStaff Search Engineer - Grapevine (AI)Liva AIFounding EngineerNovoflowFounding Software EngineerSuperKalamFullstack Engineer (internship)Veryfi, Inc.Senior Python EngineerInstrumentlSenior Full-Stack EngineerSmartAssetSenior Software EngineerAON3DSenior Frontend Engineer - PlatformDench.comFounding EngineerCoLoopSenior Fullstack EngineerOpenFunnelFounding Full Stack Engineer (including AI)PrelimSoftware EngineerSully.aiHead of Engineering, QABetter AuthStaff EngineerCobaCoba.ai Hiring | Full-stack developers for US-MX cross-border fintech (remote US or MX)Simple AIForward Deployed Software EngineerSieveDistributed Systems EngineerSoffFull-Stack EngineerHeraFounding Software EngineerFooterY CombinatorProgramsYC ProgramStartup SchoolWork at a StartupCo-Founder MatchingCompanyYC BlogContactPressPeopleCareersPrivacy PolicyNotice at CollectionSecurityTerms of UseResourcesStartup DirectoryStartup LibraryInvestorsSAFEHacker NewsLaunch YCYC DealsMake something people want.ApplyTwitterTwitterFacebookFacebookInstagramInstagramLinkedInLinkedInYoutubeYouTube©2025Y Combinator</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Django</t>
+          <t>AWS, Azure, CI/CD, Django, Docker, Google Cloud, Kubernetes</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>https://www.ycombinator.com/companies/verge-genomics/jobs/0yOYWFC-principal-full-stack-engineer-django</t>
+          <t>https://www.ycombinator.com/companies/verge-genomics/jobs/yhxsJF8-senior-data-engineer</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-10-24T15:02:33.608655</t>
+          <t>2025-10-24T15:40:39.799034</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>837645413c79e6fd58c978f58104b5cc3885d425ca0d12a732cdadf54aebde09</t>
+          <t>43437c1147e05629b0d7444a7a97c70fbcd465058df4f339deb4c6fd9b795075</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -553,7 +557,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Head of Product &amp; Engineering</t>
+          <t>Principal Full-Stack Engineer (Django)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -561,22 +565,26 @@
           <t>San Francisco - Remote / Remote (US)</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>AboutWhat Happens at YC?ApplyYC Interview GuideFAQPeopleYC BlogCompaniesStartup DirectoryFounder DirectoryLaunch YCStartup JobsAll Jobs◦ Engineering◦ Operations◦ Marketing◦ SalesInternshipsStartup Job GuideYC Startup Jobs BlogFind a Co-FounderLibrarySAFEResourcesStartup SchoolNewsletterRequests for StartupsFor InvestorsVerify FoundersHacker NewsBookfaceOpen main menuApply forW2026batch.ApplyVerge GenomicsWe use human data and AI to develop better drugs faster.Principal Full-Stack Engineer (Django)•San Francisco - Remote / Remote (US)Job typeFull-timeRoleEngineering, Full stackVisaUS citizen/visa onlyApply toVerge Genomicsand hundreds of other fast-growing YC startups with a single profile.Apply to role ›About the roleWho We AreTechnology has transformed every aspect of our lives. Yet, it still takes 12 years to develop a single drug because 90% of drugs fail in clinical trials, leaving hundreds of millions of patients without effective treatments. Accelerating the pace of bringing new, effective medicines to patients is one of the greatest opportunities for humanity.Our mission is to develop better drugs, faster using artificial intelligence (AI) and human data. We have created a proprietary, all-in-human AI drug discovery engine, CONVERGE, which houses one of the field's largest and most comprehensive databases of multi-modal patient data sourced directly from human tissue. We use machine learning to map the complex causes of disease, discover new targets with a greater probability of success, and de-risk drug development.We have delivered 2 new drugs from CONVERGE to clinical trials, discovered 282 new targets, and signed 2 commercial partnerships with Eli Lilly and AstraZeneca totaling $1.6B. We are a team of engineers, neuroscientists, and drug developers united around an audacious vision: to build the Genentech of the digital age.Your MissionReporting to the Head of Product &amp; Engineering, and working alongside Verge's platform and computational biology teams, the principal full-stack engineer will be responsible for writing and shipping the code that matures Verge's drug discovery engine to enable faster, easier access to data and rapid innovation for internal stakeholders, while laying the rails for Verge's third-party customers and partners to harness them directly in the future.Verge's platform team is a small, highly autonomous group of scientists, engineers, and subject matter experts. The successful candidate will play a key part in scoping and directing the priorities and technical solutions they implement.Your 12 Month OutcomesMature internal target discovery service into self-serve tool for internal stakeholdersMVP of self-serve SaaS platform built on top of internal service to allow external customers to leverage Verge's proprietary dataset and tools.You Will OwnDesign and build user-facing web applications that transform data platform outputs into intuitive, self-service products for internal and external customers,Develop Django-based interfaces including views, templates, forms, and APIs that enable users to interact with underlying data and analysis,Create interactive dashboards, data visualization tools, and exploration interfaces that make complex data accessible to non-technical users,Collaborate with the Data Engineer to understand data structures, APIs, and pipeline outputs, translating them into compelling user experiences,Build authentication, authorisation, and user management systems to support multi-tenant SaaS operationsImplement customer onboarding flows, account management interfaces, and self-service configuration toolsIntegrate charting and visualization libraries (D3.js, Chart.js, Plotly) to produce scientifically accurate and user-friendly data displays,Build RESTful APIs and backend services that connect Django applications to the underlying data platform,Participate in user testing and gather feedback to iteratively improve product usability and feature set,Establish automated testing frameworks and CI/CD pipelines for reliable deployments,Monitor application performance, user behaviour analytics, and error tracking to identify improvement opportunities,Work cross-functionally with science, engineering, and commercial teams to prioritise features and gather requirements.RequirementsCandidatesmust have:Either:7+ years of professional experience building web applications as a full-stack engineer, with extensive experience of Django,Extensive experience with frontend frameworks or libraries (React, Vue, or similar),Significant experience using data visualization libraries (D3.js, Chart.js, Plotly, etc.) to create impactful charts and dashboards for a variety of user stories,Deep understanding of the pros and cons of different databases for different use cases, and strong opinions on abstractions such as GraphQL and SQLAlchemy,Mastery of version control (Git), testing frameworks such as Pytest and Jest, and CI/CD pipelines,Professional fluency with web security best practices (CSRF, XSS, authentication, authorization) and state management,Demonstrable experience conceiving and implementing thoughtful user interfaces (whether hand-rolled or utilizing modern component libraries and frameworks) that help users rapidly experience the value of a service,Comfortable translating technical capabilities and internal functionality into user-facing features and benefits,Deep playbook for collaborating with both technical (e.g. data engineers, scientists) and non-technical (e.g. business development) stakeholdersAbility to thrive in uncertainty with frequently changing prioritiesDeep alignment with&lt;u&gt; our values&lt;/u&gt;A passion for making an impact on patientsExceptional candidatesmay also have:Previous experience building SaaS products or multi-tenant web applications,Knowledge of modern CSS frameworks and component libraries,Extensive experience with web sockets or other real-time data streaming technologies in a web application context,Familiarity with the challenges of, and approaches to, working with data-intensive applications or scientific software,Experience working with cloud platforms (AWS, GCP, Azure) and containerization (Docker),Working knowledge of user analytics tools (Mixpanel, Amplitude, Google Analytics),Previous experience collaborating with scientific or technical end-users.Finally, we seek candidates who embrace our values and way of working:Ability to thrive in uncertainty with frequently changing prioritiesDeep alignment withour valuesA passion for making an impact on patientsAboutVerge GenomicsTechnology has transformed every aspect of our lives. Yet, it still takes 12 years to develop a single drug because 90% of drugs fail in clinical trials, leaving hundreds of millions of patients without effective treatments. Accelerating the pace of bringing new, effective medicines to patients is one of the greatest opportunities for humanity.Our mission is to develop better drugs, faster using artificial intelligence (AI) and human data. We have created a proprietary, all-in-human AI drug discovery engine, CONVERGE, which houses one of the field's largest and most comprehensive databases of multi-modal patient data sourced directly from human tissue. We use machine learning to map the complex causes of disease, discover new targets with a greater probability of success, and de-risk drug development.We have delivered 2 new drugs from CONVERGE to clinical trials, discovered 282 new targets, and signed 2 commercial partnerships with Eli Lilly and AstraZeneca totaling $1.6B. We are a team of engineers, neuroscientists, and drug developers united around an audacious vision: to build the Genentech of the digital age.Verge GenomicsFounded:2015Batch:S15Team Size:50Status:ActiveFoundersAlice ZhangCEOAlice ZhangCEOSimilar JobsEkhoFull-stack EngineerGatherStaff Search Engineer - Grapevine (AI)Liva AIFounding EngineerNovoflowFounding Software EngineerSuperKalamFullstack Engineer (internship)Veryfi, Inc.Senior Python EngineerInstrumentlSenior Full-Stack EngineerSmartAssetSenior Software EngineerAON3DSenior Frontend Engineer - PlatformDench.comFounding EngineerCoLoopSenior Fullstack EngineerOpenFunnelFounding Full Stack Engineer (including AI)PrelimSoftware EngineerSully.aiHead of Engineering, QABetter AuthStaff EngineerCobaCoba.ai Hiring | Full-stack developers for US-MX cross-border fintech (remote US or MX)Simple AIForward Deployed Software EngineerSieveDistributed Systems EngineerSoffFull-Stack EngineerHeraFounding Software EngineerFooterY CombinatorProgramsYC ProgramStartup SchoolWork at a StartupCo-Founder MatchingCompanyYC BlogContactPressPeopleCareersPrivacy PolicyNotice at CollectionSecurityTerms of UseResourcesStartup DirectoryStartup LibraryInvestorsSAFEHacker NewsLaunch YCYC DealsMake something people want.ApplyTwitterTwitterFacebookFacebookInstagramInstagramLinkedInLinkedInYoutubeYouTube©2025Y Combinator</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Figma, User Research, A/B Testing</t>
+          <t>AWS, Azure, CI/CD, Django, Docker, Google Cloud, Graphql</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>https://www.ycombinator.com/companies/verge-genomics/jobs/EF3iPnX-head-of-product-engineering</t>
+          <t>https://www.ycombinator.com/companies/verge-genomics/jobs/0yOYWFC-principal-full-stack-engineer-django</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-10-24T15:02:38.566356</t>
+          <t>2025-10-24T15:40:49.799975</t>
         </is>
       </c>
     </row>
@@ -606,12 +614,16 @@
           <t>United States (Remote) / Remote (US)</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>AboutWhat Happens at YC?ApplyYC Interview GuideFAQPeopleYC BlogCompaniesStartup DirectoryFounder DirectoryLaunch YCStartup JobsAll Jobs◦ Engineering◦ Operations◦ Marketing◦ SalesInternshipsStartup Job GuideYC Startup Jobs BlogFind a Co-FounderLibrarySAFEResourcesStartup SchoolNewsletterRequests for StartupsFor InvestorsVerify FoundersHacker NewsBookfaceOpen main menuApply forW2026batch.ApplyOneSignalEngage customers through personalized omni-channel messagingSenior Software Engineer, Journeys Team (Fullstack)•United States (Remote) / Remote (US)Job typeFull-timeRoleEngineering, Full stackVisaUS citizen/visa onlyApply toOneSignaland hundreds of other fast-growing YC startups with a single profile.Apply to role ›About the roleOneSignal is a leading omnichannel customer engagement solution, powering personalized customer journeys across mobile and web push notifications, in-app messaging, SMS, and email. On a mission to democratize engagement, we enable over a million businesses to keep their users - including readers, fans, players and shoppers - engaged and up to date by delivering billions of messagesdaily.1 in 5 new apps launches using OneSignal! We support companies in 140 countries, including Zynga, USA Today,Bitcoin.com, Eventbrite, Tribune, and many more - from startups and small businesses just getting off the ground to established companies communicating with millions of customers.We’re Series C, venture-backed by SignalFire, Rakuten Ventures, Y Combinator, HubSpot, and BAM Elevate. We offer remote work as the default option in the United States in California, Colorado, Massachusetts, New York, New Jersey, Oregon, Pennsylvania, Texas, Utah and Washington. As well as in the UK and Singapore - with plans to expand the locations we support in the future. Some roles are hybrid roles and will be listed as such. We have offices in San Mateo, CA and London, UK, and offer flex seating options for employees to work together in-person where we don't have offices. Hiring in Singapore is done in partnership with a local PEO.OneSignal has a lot of the great tech startup qualities you'd expect, but we don't stop there. Our massive scale and small team, emphasis on healthy life balance and kindness in all our interactions, and focus on ownership and personal growth make OneSignal a uniquely great place to work.Ourblogcontains more information about the OneSignal Engineeringcareer ladder, and ourdiverse team.About The Team:OurJourney’s teamdevelops the product our customers use to orchestrate and evaluate multi-channel user engagement campaigns across SMS, Push, Email and more. This team maintains a deep understanding of our customers’ workflows and the technical details of all the messaging channels we offer to build highly flexible, no-code solutions that enable our customers to confidently engage the right user, at the right moment, with the right message.As a Senior Software Engineer, you'll be expected to take ownership of end-to-end projects that require developing in multiple languages across the stack. Your ability to consider performance characteristics, user experience, and maintainability of systems will be critical to success in this role. Your contributions will shape the way household brand names engage with their users.What You'll Do:Collaborate with Product Managers, Designers, and Engineers to implement new features for our Customer Engagement products, using Rust, Go, Ruby and more.Conduct code and specification reviews, providing technical insights to improve our features and code baseResolve production reliability issues and ensure the system scales to meet the demands of our customersRefactor components on the frontend, creating extensible, reusable and clean component architectureStay up-to-date with the latest industry trends and technologies, incorporating new ideas into our engineering processesWhat You'll Bring:6+ years of professional software development experienceExperience working with backend distributed systems at scaleExperience with two system programming languages (Rust, C++, Go, etc)A strong willingness to learn new technologies rapidlyExperience designing RESTful and/or gRPC APIsExperience with data modeling for scale using MySQL, PostgreSQL, Redis, Cassandra, and/or ScyllaDBAbility to own and deliver end to end software functionality from design/architecture, through implementation, testing, production, release, and monitoringAbility to manage complex cross-team coordination and work closely with product ownersAbility to evaluate and communicate different engineering solutions and trade-offsWe value a variety of experiences, and these are not required. It would be an added bonus if you have experience in any of the following:Experience with Rust or Ruby at scale in production environmentsExperience with event streaming framework such as Apache KafkaExperience with OpenTelemetry, Grafana and monitoring distributed systemsExperience with BI tools such as Superset, Tableau, etcExperience with KubernetesStrong Opinions on Testing MethodologiesOpen Source code maintainershipThe New York and California base salary for Senior Software Engineer full time position is between $170,000 to $190,000. Your exact starting salary is determined by a number of factors such as your experience, skills, and qualifications. In addition to base salary, we also offer a competitive equity program and comprehensive and inclusive benefits.Qualities we look for:Friendliness &amp; EmpathyAccountability &amp; CollaborationProactiveness &amp; UrgencyGrowth Mindset &amp; Love of LearningIn keeping with our beliefs and goals, no employee or applicant will face discrimination/harassment based on: race, color, ancestry, national origin, religion, age, gender, marital domestic partner status, sexual orientation, gender identity, disability status, or veteran status. Above and beyond discrimination/harassment based on 'protected categories,' we also strive to prevent other, subtler forms of inappropriate behavior (e.g., stereotyping) from ever gaining a foothold in our office. Whether blatant or hidden, barriers to success have no place in our workplace.Applicants with disabilities may be entitled to reasonable accommodation under the terms of the Americans with Disabilities Act and certain state or local laws. A reasonable accommodation is a change in the way things are normally done which will ensure an equal employment opportunity without imposing undue hardship on OneSignal. Please inform us if you need assistance completing any forms or to otherwise participate in the application and/or interview process.OneSignal collects and processes personal data submitted by job applicants in accordance with ourPrivacy Policy- including GDPR and CCPA compliance. Please see ourprivacy notice for job applicants.AboutOneSignalWe started as app developers who just wanted a developer-friendly API for push notifications. Finding no good solution, we built one ourselves.Today, OneSignal is the leading solution for sending effective messages across channels includingmobile push notifications,web push notifications,in-app messaging,SMS, andemail. We support over1,800,000of the world's leading marketers and developers.OneSignal is available on every platform and development environment, letting content creators focus on quality user engagement instead of complex implementation.We are growing faster than ever, and hiring in all departments. We hope you'll apply and we look forward to meeting you!OneSignalFounded:2011Batch:S11Team Size:150Status:ActiveLocation:San Mateo, CAFoundersGeorge DeglinFounder/CEOGeorge DeglinFounder/CEOLong VoCOOLong VoCOOSimilar JobsEkhoFull-stack EngineerGatherStaff Search Engineer - Grapevine (AI)Liva AIFounding EngineerNovoflowFounding Software EngineerSuperKalamFullstack Engineer (internship)Veryfi, Inc.Senior Python EngineerInstrumentlSenior Full-Stack EngineerSmartAssetSenior Software EngineerAON3DSenior Frontend Engineer - PlatformDench.comFounding EngineerCoLoopSenior Fullstack EngineerOpenFunnelFounding Full Stack Engineer (including AI)PrelimSoftware EngineerSully.aiHead of Engineering, QABetter AuthStaff EngineerCobaCoba.ai Hiring | Full-stack developers for US-MX cross-border fintech (remote US or MX)Simple AIForward Deployed Software EngineerSieveDistributed Systems EngineerSoffFull-Stack EngineerHeraFounding Software EngineerFooterY CombinatorProgramsYC ProgramStartup SchoolWork at a StartupCo-Founder MatchingCompanyYC BlogContactPressPeopleCareersPrivacy PolicyNotice at CollectionSecurityTerms of UseResourcesStartup DirectoryStartup LibraryInvestorsSAFEHacker NewsLaunch YCYC DealsMake something people want.ApplyTwitterTwitterFacebookFacebookInstagramInstagramLinkedInLinkedInYoutubeYouTube©2025Y Combinator</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>JavaScript, React, Node.js, SQL</t>
+          <t>Go, Mysql, Python, Ruby, Rust</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -621,7 +633,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-10-24T15:02:41.771988</t>
+          <t>2025-10-24T15:40:58.157335</t>
         </is>
       </c>
     </row>
@@ -651,12 +663,16 @@
           <t>United States (Remote) / Remote (US)</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>AboutWhat Happens at YC?ApplyYC Interview GuideFAQPeopleYC BlogCompaniesStartup DirectoryFounder DirectoryLaunch YCStartup JobsAll Jobs◦ Engineering◦ Operations◦ Marketing◦ SalesInternshipsStartup Job GuideYC Startup Jobs BlogFind a Co-FounderLibrarySAFEResourcesStartup SchoolNewsletterRequests for StartupsFor InvestorsVerify FoundersHacker NewsBookfaceOpen main menuApply forW2026batch.ApplyOneSignalEngage customers through personalized omni-channel messagingStaff Software Engineer, SMS Team (Fullstack)•United States (Remote) / Remote (US)Job typeFull-timeRoleEngineering, Full stackVisaUS citizen/visa onlyApply toOneSignaland hundreds of other fast-growing YC startups with a single profile.Apply to role ›About the roleOneSignal is a leading omnichannel customer engagement solution, powering personalized customer journeys across mobile and web push notifications, in-app messaging, SMS, and email. On a mission to democratize engagement, we enable over a million businesses to keep their users - including readers, fans, players and shoppers - engaged and up to date by delivering billions of messagesdaily.1 in 5 new apps launches using OneSignal! We support companies in 140 countries, including Zynga, USA Today,Bitcoin.com, Eventbrite, Tribune, and many more - from startups and small businesses just getting off the ground to established companies communicating with millions of customers.We’re Series C, venture-backed by SignalFire, Rakuten Ventures, Y Combinator, HubSpot, and BAM Elevate. We offer remote work as the default option in the United States in California, Colorado, Massachusetts, New York, New Jersey, Oregon, Pennsylvania, Texas, Utah and Washington. As well as in the UK and Singapore - with plans to expand the locations we support in the future. Some roles are hybrid roles and will be listed as such. We have offices in San Mateo, CA and London, UK, and offer flex seating options for employees to work together in-person where we don't have offices. Hiring in Singapore is done in partnership with a local PEO.OneSignal has a lot of the great tech startup qualities you'd expect, but we don't stop there. Our massive scale and small team, emphasis on healthy life balance and kindness in all our interactions, and focus on ownership and personal growth make OneSignal a uniquely great place to work.Ourblogcontains more information about the OneSignal Engineeringcareer ladder, and ourdiverse team.About The Team:The SMS team at OneSignal develops the UI and API powering our market leading text messaging customer engagement solution. The team tackles challenges at the intersection of engineering and product development, solving complex problems such as global quiet hours compliance across 40 time zones, and conversational text messaging in the age of AI.We’re continually improving our product to enhance our customers’ experience and empower them to create effective and impactful messaging campaigns. We move quickly on delivering value to our customers, while maintaining a high standard for reliability and functionality.As a Staff Software Engineer, you'll be expected to take ownership of end-to-end projects that require developing in multiple languages across the stack. Your ability to consider performance characteristics, user experience, and maintainability of systems will be critical to success in this role. Your contributions will shape the way household brand names engage with their users. You will drive organizational proficiencies in key technologies and technical areas, such as scalable architecture and programming language expertisWhat You'll Do:Collaborate with Product Managers, Designers, and Engineers to implement new features for our Customer Engagement products, using Rust, TypeScript, and Ruby.Conduct code and specification reviews, providing technical insights to improve our features and code baseResolve production reliability issues and ensure the system scales to meet the demands of our customersRefactor components on the frontend, creating extensible, reusable and clean component architectureStay up-to-date with the latest industry trends and technologies, incorporating new ideas into our engineering processesPresent Technical Specifications to other Staff Engineers, drive alignment on proposed solutions, and prototype draft implementationsWhat You'll Bring:8+ years of professional software development experienceExperience creating extensible, reusable React componentsExperience with TypeScript and at least one system programming language (Rust, Go, Ruby, etc)Experience working with backend distributed systems at scaleAbility to own and deliver end to end software functionality from design/architecture, through implementation, testing, production, release, and monitoringAbility to manage complex cross-team coordination and work closely with product ownersAbility to evaluate and communicate different engineering solutions and trade-offsA strong willingness to learn new technologies rapidlyExperience designing RESTful and/or gRPC APIsWe value a variety of experiences, and these are not required. It would be an added bonus if you have experience in any of the following:Experience with event streaming framework such as Apache KafkaExperience with Rust or another systems programming languageExperience with KubernetesExperience with data modeling using at least one database engine (MySQL, PostgreSQL, Redis, Cassandra, ScyllaDB, etc.)The New York and California base salary for Staff Software Engineer full time position is between $190,000 and $210,000. Your exact starting salary is determined by a number of factors such as your experience, skills, and qualifications. In addition to base salary, we also offer a competitive equity program and comprehensive and inclusive benefits.Qualities we look for:Friendliness &amp; EmpathyAccountability &amp; CollaborationProactiveness &amp; UrgencyGrowth Mindset &amp; Love of LearningIn keeping with our beliefs and goals, no employee or applicant will face discrimination/harassment based on: race, color, ancestry, national origin, religion, age, gender, marital domestic partner status, sexual orientation, gender identity, disability status, or veteran status. Above and beyond discrimination/harassment based on 'protected categories,' we also strive to prevent other, subtler forms of inappropriate behavior (e.g., stereotyping) from ever gaining a foothold in our office. Whether blatant or hidden, barriers to success have no place in our workplace.Applicants with disabilities may be entitled to reasonable accommodation under the terms of the Americans with Disabilities Act and certain state or local laws. A reasonable accommodation is a change in the way things are normally done which will ensure an equal employment opportunity without imposing undue hardship on OneSignal. Please inform us if you need assistance completing any forms or to otherwise participate in the application and/or interview process.OneSignal collects and processes personal data submitted by job applicants in accordance with ourPrivacy Policy- including GDPR and CCPA compliance. Please see ourprivacy notice for job applicants.AboutOneSignalWe started as app developers who just wanted a developer-friendly API for push notifications. Finding no good solution, we built one ourselves.Today, OneSignal is the leading solution for sending effective messages across channels includingmobile push notifications,web push notifications,in-app messaging,SMS, andemail. We support over1,800,000of the world's leading marketers and developers.OneSignal is available on every platform and development environment, letting content creators focus on quality user engagement instead of complex implementation.We are growing faster than ever, and hiring in all departments. We hope you'll apply and we look forward to meeting you!OneSignalFounded:2011Batch:S11Team Size:150Status:ActiveLocation:San Mateo, CAFoundersGeorge DeglinFounder/CEOGeorge DeglinFounder/CEOLong VoCOOLong VoCOOSimilar JobsEkhoFull-stack EngineerGatherStaff Search Engineer - Grapevine (AI)Liva AIFounding EngineerNovoflowFounding Software EngineerSuperKalamFullstack Engineer (internship)Veryfi, Inc.Senior Python EngineerInstrumentlSenior Full-Stack EngineerSmartAssetSenior Software EngineerAON3DSenior Frontend Engineer - PlatformDench.comFounding EngineerCoLoopSenior Fullstack EngineerOpenFunnelFounding Full Stack Engineer (including AI)PrelimSoftware EngineerSully.aiHead of Engineering, QABetter AuthStaff EngineerCobaCoba.ai Hiring | Full-stack developers for US-MX cross-border fintech (remote US or MX)Simple AIForward Deployed Software EngineerSieveDistributed Systems EngineerSoffFull-Stack EngineerHeraFounding Software EngineerFooterY CombinatorProgramsYC ProgramStartup SchoolWork at a StartupCo-Founder MatchingCompanyYC BlogContactPressPeopleCareersPrivacy PolicyNotice at CollectionSecurityTerms of UseResourcesStartup DirectoryStartup LibraryInvestorsSAFEHacker NewsLaunch YCYC DealsMake something people want.ApplyTwitterTwitterFacebookFacebookInstagramInstagramLinkedInLinkedInYoutubeYouTube©2025Y Combinator</t>
+        </is>
+      </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
-          <t>JavaScript, React, Node.js, SQL</t>
+          <t>Go, Mysql, Python, React, Ruby, Rust, Typescript</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -666,14 +682,14 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-10-24T15:02:47.576364</t>
+          <t>2025-10-24T15:41:09.155060</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3bca187ff3070cb30b9cf826897b761d64976d6df0f525d7dd8185a72f774fd8</t>
+          <t>0fc661e4a4fea41cae81042e5723e50a6ad40df292b11dbb01d6cad0452a168f</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -688,30 +704,26 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Web Design Engineer</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Hybrid in Santa Clara, CA</t>
-        </is>
-      </c>
+          <t>HackerRank (YC S11) is Hiring a Senior Software Engineer Fullstack</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>TypeScript, React, CSS, Design Systems</t>
+          <t>JavaScript, React, Node.js, SQL</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>https://www.ycombinator.com/companies/hackerrank/jobs/HFH0zad-web-design-engineer</t>
+          <t>https://www.ycombinator.com/companies/hackerrank/jobs/jk6xfKz-hackerrank-yc-s11-is-hiring-a-senior-software-engineer-fullstack</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-10-24T15:02:51.117003</t>
+          <t>2025-10-24T15:41:18.589271</t>
         </is>
       </c>
     </row>
@@ -741,7 +753,11 @@
           <t>Santa Clara, CA, US</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>$210 - $246</t>
+        </is>
+      </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
@@ -756,7 +772,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2025-10-24T15:02:54.750874</t>
+          <t>2025-10-24T15:41:27.107572</t>
         </is>
       </c>
     </row>
@@ -786,7 +802,11 @@
           <t>San Francisco / Remote (US; CA; MX; CO; AR; BR; PE)</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>$125K - $225K</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr">
@@ -801,7 +821,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2025-10-24T15:02:57.559126</t>
+          <t>2025-10-24T15:41:37.556473</t>
         </is>
       </c>
     </row>
@@ -831,7 +851,11 @@
           <t>US / CA / MX / BR / AR / CO / PE / Remote (US; CA; MX; BR; AR; CO; PE)</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>$125K - $225K</t>
+        </is>
+      </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr">
@@ -846,7 +870,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2025-10-24T15:03:01.941091</t>
+          <t>2025-10-24T15:41:48.067004</t>
         </is>
       </c>
     </row>
@@ -876,7 +900,11 @@
           <t>San Francisco, CA, US</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>We're Robinhood for pre-IPO startups. Everyone can invest $100.</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr">
@@ -891,14 +919,14 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2025-10-24T15:03:06.838037</t>
+          <t>2025-10-24T15:41:54.955957</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>963e3770bc59028c8b36e775e0701522592bbe4612dbde88798bc6ba685e94cb</t>
+          <t>0f0ba697990f093214443523f8e1d62fd8d42be5604da45d1e2b15017a0cef0a</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -913,33 +941,41 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Full-Stack Robotics Engineer Summer 2026 Intern</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+          <t>Computer Vision Engineer</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>UK / Remote (US)</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>AboutWhat Happens at YC?ApplyYC Interview GuideFAQPeopleYC BlogCompaniesStartup DirectoryFounder DirectoryLaunch YCStartup JobsAll Jobs◦ Engineering◦ Operations◦ Marketing◦ SalesInternshipsStartup Job GuideYC Startup Jobs BlogFind a Co-FounderLibrarySAFEResourcesStartup SchoolNewsletterRequests for StartupsFor InvestorsVerify FoundersHacker NewsBookfaceOpen main menuApply forW2026batch.ApplyCircuitHubOn-Demand Electronics ManufacturingComputer Vision Engineer£80K - £150K GBP•0.10% - 0.25%•UK / Remote (US)Job typeFull-timeRoleEngineering, Full stackExperienceAny (new grads ok)VisaUS citizen/visa onlySkillsTorch/PyTorch, OpenCVApply toCircuitHuband hundreds of other fast-growing YC startups with a single profile.Apply to role ›About the roleAbout CircuitHubCircuitHub is reshaping electronics manufacturing withThe Grid, a factory-scale robotics platform designed to make small-batch, high-mix electronics assembly radically more efficient. Think semiconductor-fab levels of precision applied to the chaotic world of prototyping and low-volume production. The result? A10x throughput improvementin one of the world's most foundational industries.We've raised$20Mfrom top-tier investors, includingY CombinatorandGoogle Ventures, and we're alreadyprofitable. Our customers include industry leaders likeTesla, Meta,andZipline.The Grid isn't a prototype. It's live, scaling fast, and delivering real revenue. We're now building the engineering core that will scale it further.What We're Looking ForWe’re looking for an engineer to found ourcomputer visionteam. We currently deploy a variety of learned models for circuit board defect detection and bin picking. We are looking for a founding engineer to architect our labelling pipeline and improve and expand the range of deployed models. This is an incredibly high-impact role that will directly contribute to 3x revenue growth over the next year.Who This Role Is ForThis role would suit a full-stack computer vision engineer comfortable building front-end labelling tools and training models. This is not a pure research position.Example TasksDecide what data we should be capturing about PCB defectsDesign and implement a database schema and front-end labelling toolTrain vision models using the labelled dataLocationRemote or work from one of our labs in the UK (London, Cambridge) or USA (Boston)Why This Role MattersThe work of the computer vision team will be critical to making electronics manufacturing economically viable in the USA and Europe. This is acareer-defining opportunityfor a high-agency engineer. If you thrive on ownership and solving real problems using advanced research techniques, there’s no better place to be.Key Tools &amp; TechnologiesPythonTypeScript and ReactOpenCVPyTorchWant to help us build the future of manufacturing?AboutCircuitHubWe're building a future where hardware companies can design and iterate as fast as software companiesCircuitHub is on a mission to fix rapid electronics prototyping. We are the first automated electronics factory built around a modern tech stack. We help hardware companies producing self driving cars, satellites, 3D printers, robotics, &amp; more to rapidly prototype electronics and get to market faster.We've raised $20M from top investors that include Y Combinator , Google Ventures, &amp; more. With business growing fast we are looking to fill roles in Massachusetts, USA and London, UK .Join us to solve real world problems while shaping the future of automated manufacturing.CircuitHubFounded:2012Batch:W12Team Size:58Status:ActiveLocation:London, United KingdomFoundersAndrew SeddonCEOAndrew SeddonCEOSimilar JobsEkhoFull-stack EngineerGatherStaff Search Engineer - Grapevine (AI)Liva AIFounding EngineerNovoflowFounding Software EngineerSuperKalamFullstack Engineer (internship)Veryfi, Inc.Senior Python EngineerInstrumentlSenior Full-Stack EngineerSmartAssetSenior Software EngineerAON3DSenior Frontend Engineer - PlatformDench.comFounding EngineerCoLoopSenior Fullstack EngineerOpenFunnelFounding Full Stack Engineer (including AI)PrelimSoftware EngineerSully.aiHead of Engineering, QABetter AuthStaff EngineerCobaCoba.ai Hiring | Full-stack developers for US-MX cross-border fintech (remote US or MX)Simple AIForward Deployed Software EngineerSieveDistributed Systems EngineerSoffFull-Stack EngineerHeraFounding Software EngineerFooterY CombinatorProgramsYC ProgramStartup SchoolWork at a StartupCo-Founder MatchingCompanyYC BlogContactPressPeopleCareersPrivacy PolicyNotice at CollectionSecurityTerms of UseResourcesStartup DirectoryStartup LibraryInvestorsSAFEHacker NewsLaunch YCYC DealsMake something people want.ApplyTwitterTwitterFacebookFacebookInstagramInstagramLinkedInLinkedInYoutubeYouTube©2025Y Combinator</t>
+        </is>
+      </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
         <is>
-          <t>JavaScript, React, Node.js, SQL</t>
+          <t>Python, Pytorch</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>https://www.ycombinator.com/companies/circuithub/jobs/pxHqv58-full-stack-robotics-engineer-summer-2026-intern</t>
+          <t>https://www.ycombinator.com/companies/circuithub/jobs/js2U2cL-computer-vision-engineer</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2025-10-24T15:03:12.247985</t>
+          <t>2025-10-24T15:42:04.650390</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>e02823e51eea2a32d60bf0380f319b2c11739b7f163e96222354cef208337faf</t>
+          <t>b4e4836c7f94a46e93e069cc22ccc236d554cf247e0a6c9855484acc7dadfa6d</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -954,15 +990,19 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Operations Research Engineer</t>
+          <t>Full-Stack Robotics Engineer</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>UK / Remote (US)</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
+          <t>Deerfield, MA, US / Remote (US)</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>$140K - $250K</t>
+        </is>
+      </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
@@ -972,19 +1012,19 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>https://www.ycombinator.com/companies/circuithub/jobs/UM1QSjZ-operations-research-engineer</t>
+          <t>https://www.ycombinator.com/companies/circuithub/jobs/bUPM5eq-full-stack-robotics-engineer</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2025-10-24T15:03:18.421095</t>
+          <t>2025-10-24T15:42:13.478400</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>98d8c8bb67db752cafbb5cce832cdcf3e5586aaf82ec3f4a7abe3a26231e153a</t>
+          <t>041208e5a6b9cbabfe8f3996b11ffe1ac42267169adad9c3ad9df530a1d1155d</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -999,7 +1039,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Staff Product Engineer, AI Agents</t>
+          <t>Senior Product Engineer, AI Agents</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1007,7 +1047,11 @@
           <t>San Francisco, CA, US</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>$203K - $305K</t>
+        </is>
+      </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
@@ -1017,12 +1061,12 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>https://www.ycombinator.com/companies/amplitude/jobs/byPftTK-staff-product-engineer-ai-agents</t>
+          <t>https://www.ycombinator.com/companies/amplitude/jobs/w0WSIC8-senior-product-engineer-ai-agents</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2025-10-24T15:03:22.660028</t>
+          <t>2025-10-24T15:42:22.482675</t>
         </is>
       </c>
     </row>
@@ -1052,7 +1096,11 @@
           <t>San Francisco, CA, US</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>$177K - $266K</t>
+        </is>
+      </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr">
@@ -1067,7 +1115,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2025-10-24T15:03:26.676450</t>
+          <t>2025-10-24T15:42:28.650193</t>
         </is>
       </c>
     </row>
@@ -1097,7 +1145,11 @@
           <t>San Francisco, CA, US</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>$140K - $180K</t>
+        </is>
+      </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
@@ -1112,14 +1164,14 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2025-10-24T15:03:31.557447</t>
+          <t>2025-10-24T15:42:37.811205</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>775a6269ac5912451c4fce93320250cfa2af9b4a5d7be9c24037df7dd82e9e1b</t>
+          <t>8c6d110e26f7c80946ee24ceb060a528db01dd48cd84a6476c7de4daed0983b4</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1134,33 +1186,37 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Founding AI Engineer</t>
+          <t>Founding Software Engineer</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>(about 4 hours ago)</t>
+        </is>
+      </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Python, TensorFlow, Model Evaluation</t>
+          <t>JavaScript, React, Node.js, SQL</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://www.ycombinator.com/companies/hera-video/jobs/itTRHs0-founding-ai-engineer</t>
+          <t>https://www.ycombinator.com/companies/hera-video/jobs/sHCLYOi-founding-software-engineer</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>2025-10-24T15:03:34.392841</t>
+          <t>2025-10-24T15:42:43.596945</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>8c6d110e26f7c80946ee24ceb060a528db01dd48cd84a6476c7de4daed0983b4</t>
+          <t>775a6269ac5912451c4fce93320250cfa2af9b4a5d7be9c24037df7dd82e9e1b</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1175,26 +1231,30 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Founding Software Engineer</t>
+          <t>Founding AI Engineer</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>AboutWhat Happens at YC?ApplyYC Interview GuideFAQPeopleYC BlogCompaniesStartup DirectoryFounder DirectoryLaunch YCStartup JobsAll Jobs◦ Engineering◦ Operations◦ Marketing◦ SalesInternshipsStartup Job GuideYC Startup Jobs BlogFind a Co-FounderLibrarySAFEResourcesStartup SchoolNewsletterRequests for StartupsFor InvestorsVerify FoundersHacker NewsBookfaceOpen main menuApply forW2026batch.ApplyHeraAI Motion DesignerFounding AI Engineer€80K - €130K EUR•0.75% - 1.50%•Berlin, BE, DE / Berlin, Berlin, DEJob typeFull-timeRoleEngineering, Machine learningExperience3+ yearsVisaUS citizenship/visa not requiredConnect directly with founders of the best YC-funded startups.Apply to role ›Peter TribelhornCo-FounderPeter TribelhornCo-FounderAbout the roleFounding AI Engineer at Hera (YC S25)We're building the world's first AI motion designer that creates professional animations in seconds.About HeraVideo is the most effective medium, but video creators waste countless hours animating seconds of content. Motion design tools like After Effects require mastering complex user interfaces, turning creative work into button-clicking hell. We're starting with motion design because it's the most painful and expensive part of video creation.Hera is the first AI motion designer that creates professional animations through conversation. Unlike video-gen tools, Hera generates code-based animations where every parameter can be fine-tuned through prompts or on-canvas editing, giving users the control of After Effects with the simplicity of Lovable.In our first two weeks after launch, users created over 200,000 animations.Our founders:Peter Tribelhorn (CEO) built YouTube channels with 50B+ views. Chia-Lun Wu (CTO) was one of the first developers at Vyond, where he built their video editor used by 20,000 businesses today.About the RoleBuild and optimize AI systems to generate high-quality animations that follow core motion design principles (easing, non-linear movement, visual hierarchy)Develop comprehensive evaluation frameworks to assess animation quality, combining automated metrics with expert validation from motion designersPartner with motion designers and marketers to translate professional design knowledge into AI training data and evaluation criteriaDesign and implement fine-tuning pipelines that teach Hera domain-specific animation styles and brand guidelinesCreate feedback loops between user preferences, expert input, and model performance to continuously improve animation qualityResearch and prototype state-of-the-art approaches for controllable, style-consistent motion graphics generationTech StackOur technology choices evolve with our needs. Current core technologies include TypeScript, React.js, Next.js, PostgreSQL, GCP/AWS, and our proprietary motion graphics engine. We prioritize learning velocity, end-to-end delivery, and adopt new languages or frameworks when they best serve our users and product goals.What Makes You a Great FitYou're hungry.Not just ambitious, but obsessed with building something massiveYou're entrepreneurial.You've built things before and demand ownershipYou thrive in ambiguity.No roadmaps, no PMs, just problems to solveYou have a growth mindset.We're small today, but building something huge. To grow the company, each of us needs to grow personallyYou work like an athlete.High performance, consistent improvement, whatever it takes to winYou want to work in-person in Berlin(we help you relocate if needed)We hire for slope, not intercept.We don't care about credentials; we care about trajectoryYou're NOT a Good Fit If:You're picky about what you work onYou lack curiosity or the hunger to learnYou prefer structured environments with clear boundariesYou think AI is just hypeYou want to specialize in one technologyWhy Hera?We're building this team like Real Madrid: small, elite, with each person being a superstar. We believe we can reach $100M ARR with less than 20 people. As a founding engineer, you'll have:Life-changing equity stakeAbove-market salaryBuild a product used by thousands dailyThe chance to redefine how millions of users create videoOffice in Berlin Mitte (1 minute from Rosa-Luxemburg-Platz)All meals on us - we serve lunch and dinner 6 days/weekAboutHeraHera (YC S25) is your AI motion designer that creates professional animations in seconds.Video teams waste countless hours animating seconds of content. Motion design tools like After Effects require mastering complex user interfaces, turning creative work into button-clicking hell.Hera is the first AI motion designer that creates professional animations through conversation. Unlike video-gen tools, Hera generates code-based animations where every parameter can be fine-tuned through prompts or on-canvas editing, giving users the control of After Effects with the simplicity of Lovable.Hera has grown to a 6-figure ARR in less than 10 days after launching publicly.HeraFounded:2025Batch:S25Team Size:2Status:ActiveFoundersPeter TribelhornCo-FounderPeter TribelhornCo-FounderChia-Lun WuFounderChia-Lun WuFounderSimilar JobsTuring Labs Inc.AI Engineer Intern - build stealth modelZeroEntropyMachine Learning Engineering Intern (Fall 2025)NanoNetsSenior Deep Learning EngineerThe Forecasting CompanyFounding Machine Learning EngineerBindwellFounding Machine Learning EngineerInferDeep Learning InternRunRLFounding EngineeriSono HealthComputer Vision/Deep Learning ScientistMbodi AIFounding Research EngineerOnyxMachine Learning EngineerBrowser UseSoftware EngineerDraftaidSenior ML EngineerClosureFounding AI EngineerStreamMachine Learning EngineerHightouchMachine Learning Engineer, AI DecisioningStripeMachine Learning Engineer, IdentityTerra APIAI EngineerQuickchat AIMachine Learning Engineer InternAnthrogenMember of Technical Staff (applied)SkywaysSenior ML/AI/CV Software EngineerFooterY CombinatorProgramsYC ProgramStartup SchoolWork at a StartupCo-Founder MatchingCompanyYC BlogContactPressPeopleCareersPrivacy PolicyNotice at CollectionSecurityTerms of UseResourcesStartup DirectoryStartup LibraryInvestorsSAFEHacker NewsLaunch YCYC DealsMake something people want.ApplyTwitterTwitterFacebookFacebookInstagramInstagramLinkedInLinkedInYoutubeYouTube©2025Y Combinator</t>
+        </is>
+      </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr">
         <is>
-          <t>JavaScript, React, Node.js, SQL</t>
+          <t>AWS, Deep Learning, Google Cloud, Machine Learning, React, Typescript</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.ycombinator.com/companies/hera-video/jobs/sHCLYOi-founding-software-engineer</t>
+          <t>https://www.ycombinator.com/companies/hera-video/jobs/itTRHs0-founding-ai-engineer</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2025-10-24T15:03:37.374690</t>
+          <t>2025-10-24T15:42:53.571233</t>
         </is>
       </c>
     </row>
@@ -1224,7 +1284,11 @@
           <t>Boulder, CO, US / Mission Viejo, CA, US / New York, NY, US / Remote (US)</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>$150K</t>
+        </is>
+      </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr">
@@ -1239,7 +1303,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2025-10-24T15:03:40.220840</t>
+          <t>2025-10-24T15:43:02.541345</t>
         </is>
       </c>
     </row>
@@ -1265,7 +1329,11 @@
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>$180K - $220K</t>
+        </is>
+      </c>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr">
@@ -1280,7 +1348,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2025-10-24T15:03:43.012962</t>
+          <t>2025-10-24T15:43:12.663231</t>
         </is>
       </c>
     </row>
@@ -1306,7 +1374,11 @@
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>$100K - $120K</t>
+        </is>
+      </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr">
@@ -1321,7 +1393,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2025-10-24T15:03:47.452675</t>
+          <t>2025-10-24T15:43:19.882926</t>
         </is>
       </c>
     </row>
@@ -1351,7 +1423,11 @@
           <t>San Francisco, CA, US</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>$120K - $250K</t>
+        </is>
+      </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr">
@@ -1366,14 +1442,14 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2025-10-24T15:03:53.765377</t>
+          <t>2025-10-24T15:43:29.444650</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>d72825ed38e0550071d74fef28fb1d99bd6545cf0e076f0aceb989784f35a5fe</t>
+          <t>52f93c572a2e2e1f54fe695745a5c3d19a600fe37c39d3ca1cf39f6211661aa0</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1388,7 +1464,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Founding Research Engineer</t>
+          <t>Founding Engineer</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1396,7 +1472,11 @@
           <t>San Francisco, CA, US</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>$160K - $350K</t>
+        </is>
+      </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr">
@@ -1406,12 +1486,12 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://www.ycombinator.com/companies/agenthub-2/jobs/Xlqq4A8-founding-research-engineer</t>
+          <t>https://www.ycombinator.com/companies/agenthub-2/jobs/u26pbv3-founding-engineer</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2025-10-24T15:03:56.891693</t>
+          <t>2025-10-24T15:43:39.562807</t>
         </is>
       </c>
     </row>
@@ -1441,7 +1521,11 @@
           <t>San Francisco, CA, US</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>$8K - $11K / monthly</t>
+        </is>
+      </c>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr">
@@ -1456,7 +1540,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2025-10-24T15:04:02.055271</t>
+          <t>2025-10-24T15:43:45.915345</t>
         </is>
       </c>
     </row>
@@ -1486,7 +1570,11 @@
           <t>San Francisco, CA, US</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>(about 12 hours ago)</t>
+        </is>
+      </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr">
@@ -1501,7 +1589,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>2025-10-24T15:04:04.870695</t>
+          <t>2025-10-24T15:43:48.488110</t>
         </is>
       </c>
     </row>
@@ -1531,7 +1619,11 @@
           <t>San Francisco, CA, US</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>$180K - $230K</t>
+        </is>
+      </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr">
@@ -1546,14 +1638,14 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2025-10-24T15:04:09.284474</t>
+          <t>2025-10-24T15:43:58.978148</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ac94e2f31b99e80c29a77d062cc8b0b58841b8ff6ff770b3f694a0dcb1726b00</t>
+          <t>16d8bf0bcc77b850c02be02487f90ac1d53c1ae3f8a6ff2805f3b22c4f4dc0e9</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1568,7 +1660,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Member Of Technical Staff (Summer Intern)</t>
+          <t>Member Of Technical Staff (Winter Intern)</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1576,7 +1668,11 @@
           <t>San Francisco, CA, US</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>$6K - $10K / monthly</t>
+        </is>
+      </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr">
@@ -1586,19 +1682,19 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.ycombinator.com/companies/wafer/jobs/0ontUwO-member-of-technical-staff-summer-intern</t>
+          <t>https://www.ycombinator.com/companies/wafer/jobs/nvcPjYk-member-of-technical-staff-winter-intern</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2025-10-24T15:04:14.297800</t>
+          <t>2025-10-24T15:44:07.375249</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>6ad80636a9923e65926fb4793dcc2ffddc6cbf3d471c23421574550b81be121f</t>
+          <t>0d259d397483e96cddfd19a81e1c449fb63329f2b3be92266a66b962c2c9f9f7</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1613,7 +1709,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Software Engineer (Full-Stack)</t>
+          <t>Founding Software Engineer (Full-Stack)</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1621,7 +1717,11 @@
           <t>San Francisco, CA, US / San Mateo, CA, US / Palo Alto, CA, US / Menlo Park, CA, US / Redwood City, CA, US</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>$150K - $190K</t>
+        </is>
+      </c>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr">
@@ -1631,19 +1731,19 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.ycombinator.com/companies/starsling/jobs/YGCndbU-software-engineer-full-stack</t>
+          <t>https://www.ycombinator.com/companies/starsling/jobs/ZvHKf88-founding-software-engineer-full-stack</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2025-10-24T15:04:20.506982</t>
+          <t>2025-10-24T15:44:17.355636</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>0d259d397483e96cddfd19a81e1c449fb63329f2b3be92266a66b962c2c9f9f7</t>
+          <t>6ad80636a9923e65926fb4793dcc2ffddc6cbf3d471c23421574550b81be121f</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1658,7 +1758,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Founding Software Engineer (Full-Stack)</t>
+          <t>Software Engineer (Full-Stack)</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1666,7 +1766,11 @@
           <t>San Francisco, CA, US / San Mateo, CA, US / Palo Alto, CA, US / Menlo Park, CA, US / Redwood City, CA, US</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr"/>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>$150K - $190K</t>
+        </is>
+      </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr">
@@ -1676,12 +1780,12 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.ycombinator.com/companies/starsling/jobs/ZvHKf88-founding-software-engineer-full-stack</t>
+          <t>https://www.ycombinator.com/companies/starsling/jobs/YGCndbU-software-engineer-full-stack</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2025-10-24T15:04:24.764760</t>
+          <t>2025-10-24T15:44:26.302737</t>
         </is>
       </c>
     </row>
@@ -1711,12 +1815,16 @@
           <t>IN / Remote (IN)</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr"/>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>AboutWhat Happens at YC?ApplyYC Interview GuideFAQPeopleYC BlogCompaniesStartup DirectoryFounder DirectoryLaunch YCStartup JobsAll Jobs◦ Engineering◦ Operations◦ Marketing◦ SalesInternshipsStartup Job GuideYC Startup Jobs BlogFind a Co-FounderLibrarySAFEResourcesStartup SchoolNewsletterRequests for StartupsFor InvestorsVerify FoundersHacker NewsBookfaceOpen main menuApply forW2026batch.ApplyThird ChairAgents for in-house legal teamsSenior Software Engineer (Backend)₹3.8M - ₹5M INR•0.05% - 0.10%•IN / Remote (IN)Job typeFull-timeRoleEngineering, BackendExperience3+ yearsVisaUS citizenship/visa not requiredSkillsNode.js, TypeScript, PostgreSQL, Amazon Web Services (AWS)Connect directly with founders of the best YC-funded startups.Apply to role ›Shourya LalaFounderShourya LalaFounderAbout the rolePlease read before applying:• Please include a note where you answer in not more than 100 words: ‘What is the most complex backend feature you’ve developed where you were the sole or primary developer. Mention the technicals in detail and peak production load.’• Applications that don’t include the note or meet the minimum requirements will not be considered.• We review every single application and have not more than 3 rounds in the process with a decision within 14 days of applying.What makes you a good fit:• 3+ years of professional work experience developing production level Node.js/Typescript backends.• Strong experience with structured DBMSs like PostgreSQL and OLAP databases like Redshift.• Strong understanding of AWS services such as ECS, RDS, S3, CloudWatch, Elasticache.• Experience working with telemetry, CI/CD and IaaC pipelines.•Comfortable with US timezones.What makes you a great fit:• Past experience with OpenAI APIs for completions, function calling and building context aware assistants.• Past experience with Go routines.• Building multi-agent systems using frameworks like CrewAI or such.• Strong sense of cost optimization strategies, system design, and building efficient API stacks.Benefits:• Work from anywhere - We're a distributed team across multiple timezones with a focus on outputs instead of location or working hours.• Generous PTO policy.• Competitive pay bracket.• Equity at a fast growing YC backed co in a disruptive market.AboutThird ChairThird Chair(YC X25)is building AI Agents for in-house legal teams. The team comprises of 2 second-time founders with past exits.Yoavpreviously cofounded social media analytics startup Trendpop(YC W21) that scaled to 1M in ARR in 16 months building a platform that processed millions of social posts per day.Shouryapreviously cofounded a consumer finance startup Fello(YC W22) that scaled to over 2 million users and managed over 600k monthly active users and over $250,000 in monthly investments.Third Chair is building vertical AI-native workflows for legal teams that help them complete end-to-end workflows that previously required 100s of hours. This is accomplished by building SOTA AI agents that browse the web, download and collect evidence, draft letters and more. We'vegrown 88% last monthand went from0 to 100k ARR in 5 months.  More here:YC LaunchThird ChairFounded:2024Batch:X25Team Size:2Status:ActiveFoundersShourya LalaFounderShourya LalaFounderYoav ZimmermanFounderYoav ZimmermanFounderSimilar JobsButterSystems Engineer (SF)PAX MarketsFounding Software EngineerLighthouz AISenior Backend Engineer - IndiaGoGoGrandparentGoGoGrandparent (YC S16) is hiring Backend and Full-Stack EngineersOpterySenior Backend Engineer (Python + Django)PositionaleBPF &amp; Kernel EngineerTrueClaimHealthcare Integrations SpecialistJoyEngineering Leader Back-EndUnboundFounding EngineerAngleraForward Deployed EngineerRiotSoftware EngineerReboltFounding Backend Software EngineerNolocoSenior Software EngineerTamarind BioInfrastructure EngineerEverestEngineering Intern (Spring &amp; Summer 26, SF free housing)VectorShiftBackend Engineer (India)AxleStaff EngineerFurtherAISoftware Engineer - Backend/FullstackCandid HealthForward Deployed Software EngineerTerra APIBackend EngineerFooterY CombinatorProgramsYC ProgramStartup SchoolWork at a StartupCo-Founder MatchingCompanyYC BlogContactPressPeopleCareersPrivacy PolicyNotice at CollectionSecurityTerms of UseResourcesStartup DirectoryStartup LibraryInvestorsSAFEHacker NewsLaunch YCYC DealsMake something people want.ApplyTwitterTwitterFacebookFacebookInstagramInstagramLinkedInLinkedInYoutubeYouTube©2025Y Combinator</t>
+        </is>
+      </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Python, REST APIs, Postgres, Docker</t>
+          <t>AWS, CI/CD, Django, Go, Node, Python, Typescript</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -1726,7 +1834,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2025-10-24T15:04:30.132987</t>
+          <t>2025-10-24T15:44:34.116113</t>
         </is>
       </c>
     </row>
@@ -1756,7 +1864,11 @@
           <t>US / Remote (US)</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr"/>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>$6K - $10K / monthly</t>
+        </is>
+      </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr">
@@ -1771,7 +1883,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2025-10-24T15:04:33.246156</t>
+          <t>2025-10-24T15:44:42.384629</t>
         </is>
       </c>
     </row>
@@ -1801,7 +1913,11 @@
           <t>San Francisco, CA, US</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr"/>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>$120K - $200K</t>
+        </is>
+      </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="inlineStr">
@@ -1816,7 +1932,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2025-10-24T15:04:37.954115</t>
+          <t>2025-10-24T15:45:01.989065</t>
         </is>
       </c>
     </row>

</xml_diff>